<commit_message>
chore: update custom test files
</commit_message>
<xml_diff>
--- a/testdata/custom/users.xlsx
+++ b/testdata/custom/users.xlsx
@@ -16,7 +16,7 @@
     <t>id</t>
   </si>
   <si>
-    <t>type</t>
+    <t>name</t>
   </si>
   <si>
     <t>John Doe</t>
@@ -273,6 +273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -304,6 +305,9 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>